<commit_message>
Fixed codetest errors (duplication and missing)
</commit_message>
<xml_diff>
--- a/CONFIG/eLIMS_contract_analysis.xlsx
+++ b/CONFIG/eLIMS_contract_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ECAR\OCR_ECAR\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A52D63C-C1A9-4D85-B91C-BDF9E73A8A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C495A7F-5774-4A28-AD28-87364EF50195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_contract" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2314" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="942">
   <si>
     <t>ContractCode</t>
   </si>
@@ -3841,8 +3841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDABCC7-A9CF-4D80-86A3-6E2C855B569A}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4996,9 +4996,7 @@
       <c r="D64" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E64" s="1"/>
       <c r="F64" s="14" t="s">
         <v>180</v>
       </c>
@@ -5029,7 +5027,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0A49CE-5BF9-4FC3-94A4-4CD73DBB13A3}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -5425,7 +5425,7 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="22" t="s">
-        <v>99</v>
+        <v>318</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>317</v>
@@ -5592,9 +5592,7 @@
       <c r="D31" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
         <v>180</v>
       </c>

</xml_diff>

<commit_message>
Fixed a type error
</commit_message>
<xml_diff>
--- a/CONFIG/eLIMS_contract_analysis.xlsx
+++ b/CONFIG/eLIMS_contract_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ECAR\OCR_ECAR\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C495A7F-5774-4A28-AD28-87364EF50195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2B01A3-997F-4F1C-AC93-F8A914217DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_contract" sheetId="1" r:id="rId1"/>
@@ -2984,7 +2984,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -3079,11 +3079,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3121,9 +3156,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3134,11 +3166,80 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3434,18 +3535,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{308B8970-D434-49C4-AEB2-51136AB851B8}" name="Table13" displayName="Table13" ref="A1:F65" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{308B8970-D434-49C4-AEB2-51136AB851B8}" name="Table13" displayName="Table13" ref="A1:F65" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
   <autoFilter ref="A1:F65" xr:uid="{308B8970-D434-49C4-AEB2-51136AB851B8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
     <sortCondition ref="D1:D65"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9A67B5F6-82CD-4F71-A424-8E56E976F748}" name="Quotation Version" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{0688B5FA-F860-4686-99B2-F7C33CD551B6}" name="Related" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{AB5F249B-B36B-4123-BDC4-F0B4FFD70F7F}" name="Denomination" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{BDD210AF-283C-4C55-9E72-A97E87F2E155}" name="Code" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{A30E5EF7-7122-462C-9DF5-A9EF23844952}" name="Type" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{90D3C7BA-350E-41CC-A574-C3636987FAB9}" name="Name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9A67B5F6-82CD-4F71-A424-8E56E976F748}" name="Quotation Version" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{0688B5FA-F860-4686-99B2-F7C33CD551B6}" name="Related" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{AB5F249B-B36B-4123-BDC4-F0B4FFD70F7F}" name="Denomination" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{BDD210AF-283C-4C55-9E72-A97E87F2E155}" name="Code" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{A30E5EF7-7122-462C-9DF5-A9EF23844952}" name="Type" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{90D3C7BA-350E-41CC-A574-C3636987FAB9}" name="Name" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BD19236B-B873-4781-88CC-19BB6A25D2EB}" name="Table3" displayName="Table3" ref="A1:F31" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:F31" xr:uid="{BD19236B-B873-4781-88CC-19BB6A25D2EB}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{05E05A0A-EDF7-45C6-9D8E-900F933D5D45}" name="Quotation Version"/>
+    <tableColumn id="2" xr3:uid="{F077605F-A37F-424B-A1CC-650EBF6EA3AA}" name="Related"/>
+    <tableColumn id="3" xr3:uid="{DEB7BC7C-DF7B-4218-98FF-6A8642E132B1}" name="Denomination"/>
+    <tableColumn id="4" xr3:uid="{B7B72708-4894-47F6-AA3E-CEBF9E0CBC3C}" name="Code"/>
+    <tableColumn id="5" xr3:uid="{B4D8C931-225C-4BDB-99FA-F74BCA4D9D6C}" name="Type"/>
+    <tableColumn id="6" xr3:uid="{12B6B304-0D9C-4B6D-BE9B-C6412DE659F8}" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3841,8 +3957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDABCC7-A9CF-4D80-86A3-6E2C855B569A}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3854,31 +3970,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>890</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>891</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="14"/>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3892,7 +4008,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1"/>
@@ -3910,7 +4026,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1"/>
@@ -3928,7 +4044,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1"/>
@@ -3946,7 +4062,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="3"/>
@@ -3964,7 +4080,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3"/>
@@ -3982,7 +4098,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="5"/>
@@ -4000,7 +4116,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="5"/>
@@ -4018,7 +4134,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="5"/>
@@ -4036,7 +4152,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="5"/>
@@ -4054,7 +4170,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3"/>
@@ -4072,11 +4188,11 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="19"/>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -4090,7 +4206,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3"/>
@@ -4108,7 +4224,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="3"/>
@@ -4126,7 +4242,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -4144,7 +4260,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="5"/>
@@ -4162,7 +4278,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3"/>
@@ -4180,7 +4296,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1"/>
@@ -4198,7 +4314,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="1"/>
@@ -4216,7 +4332,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="1"/>
@@ -4234,7 +4350,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="1"/>
@@ -4252,7 +4368,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="1"/>
@@ -4270,7 +4386,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="1"/>
@@ -4288,7 +4404,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="1"/>
@@ -4306,7 +4422,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="1"/>
@@ -4324,7 +4440,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="1"/>
@@ -4342,7 +4458,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="1"/>
@@ -4360,7 +4476,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="7"/>
@@ -4376,7 +4492,7 @@
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="7"/>
@@ -4392,7 +4508,7 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="1"/>
@@ -4410,7 +4526,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="1"/>
@@ -4428,7 +4544,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B33" s="1"/>
@@ -4446,7 +4562,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B34" s="1"/>
@@ -4464,7 +4580,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="1"/>
@@ -4482,7 +4598,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="1"/>
@@ -4500,7 +4616,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B37" s="1"/>
@@ -4518,7 +4634,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="1"/>
@@ -4536,7 +4652,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="1"/>
@@ -4554,7 +4670,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="1"/>
@@ -4572,7 +4688,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="1"/>
@@ -4590,7 +4706,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B42" s="1"/>
@@ -4608,7 +4724,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="1"/>
@@ -4626,7 +4742,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B44" s="1"/>
@@ -4644,7 +4760,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B45" s="1"/>
@@ -4662,7 +4778,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A46" s="28" t="s">
+      <c r="A46" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B46" s="1"/>
@@ -4680,7 +4796,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B47" s="1"/>
@@ -4698,7 +4814,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B48" s="1"/>
@@ -4716,7 +4832,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B49" s="1"/>
@@ -4734,7 +4850,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B50" s="1"/>
@@ -4752,7 +4868,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B51" s="1"/>
@@ -4770,7 +4886,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B52" s="1"/>
@@ -4788,7 +4904,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A53" s="28" t="s">
+      <c r="A53" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B53" s="1"/>
@@ -4806,7 +4922,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B54" s="1"/>
@@ -4824,7 +4940,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B55" s="1"/>
@@ -4842,7 +4958,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B56" s="1"/>
@@ -4860,7 +4976,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A57" s="28" t="s">
+      <c r="A57" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B57" s="1"/>
@@ -4878,7 +4994,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B58" s="1"/>
@@ -4896,7 +5012,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A59" s="28" t="s">
+      <c r="A59" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B59" s="1"/>
@@ -4914,7 +5030,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B60" s="1"/>
@@ -4932,7 +5048,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A61" s="28" t="s">
+      <c r="A61" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B61" s="1"/>
@@ -4950,7 +5066,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A62" s="28" t="s">
+      <c r="A62" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B62" s="1"/>
@@ -4968,14 +5084,14 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B63" s="14"/>
       <c r="C63" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="D63" s="32" t="s">
+      <c r="D63" s="31" t="s">
         <v>176</v>
       </c>
       <c r="E63" s="1" t="s">
@@ -4986,14 +5102,14 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B64" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="C64" s="33"/>
-      <c r="D64" s="32" t="s">
+      <c r="C64" s="32"/>
+      <c r="D64" s="31" t="s">
         <v>179</v>
       </c>
       <c r="E64" s="1"/>
@@ -5002,18 +5118,18 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A65" s="34"/>
-      <c r="B65" s="35" t="s">
+      <c r="A65" s="33"/>
+      <c r="B65" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="C65" s="35"/>
-      <c r="D65" s="35" t="s">
+      <c r="C65" s="34"/>
+      <c r="D65" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="E65" s="35" t="s">
+      <c r="E65" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="F65" s="35"/>
+      <c r="F65" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5027,40 +5143,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0A49CE-5BF9-4FC3-94A4-4CD73DBB13A3}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="32.90625" customWidth="1"/>
+    <col min="4" max="4" width="7.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="26" t="s">
         <v>890</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="26" t="s">
         <v>891</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="39" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B2" s="1"/>
@@ -5073,12 +5189,12 @@
       <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="35" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B3" s="1"/>
@@ -5091,12 +5207,12 @@
       <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="35" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B4" s="1"/>
@@ -5109,12 +5225,12 @@
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="35" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B5" s="1"/>
@@ -5127,12 +5243,12 @@
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="35" t="s">
         <v>898</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B6" s="1"/>
@@ -5145,12 +5261,12 @@
       <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="35" t="s">
         <v>901</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="28" t="s">
         <v>892</v>
       </c>
       <c r="B7" s="3"/>
@@ -5163,12 +5279,12 @@
       <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="36" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="28" t="s">
         <v>892</v>
       </c>
       <c r="B8" s="3"/>
@@ -5181,12 +5297,12 @@
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="36" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="28" t="s">
         <v>892</v>
       </c>
       <c r="B9" s="3"/>
@@ -5199,12 +5315,12 @@
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="36" t="s">
         <v>908</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="28" t="s">
         <v>892</v>
       </c>
       <c r="B10" s="3"/>
@@ -5217,12 +5333,12 @@
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="36" t="s">
         <v>911</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="29" t="s">
         <v>892</v>
       </c>
       <c r="B11" s="5"/>
@@ -5235,12 +5351,12 @@
       <c r="E11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="37" t="s">
         <v>914</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="29" t="s">
         <v>892</v>
       </c>
       <c r="B12" s="5"/>
@@ -5253,12 +5369,12 @@
       <c r="E12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="37" t="s">
         <v>916</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="28" t="s">
         <v>892</v>
       </c>
       <c r="B13" s="3"/>
@@ -5271,12 +5387,12 @@
       <c r="E13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="36" t="s">
         <v>918</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="28" t="s">
         <v>892</v>
       </c>
       <c r="B14" s="3"/>
@@ -5289,12 +5405,12 @@
       <c r="E14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="36" t="s">
         <v>920</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="28" t="s">
         <v>892</v>
       </c>
       <c r="B15" s="3"/>
@@ -5307,12 +5423,12 @@
       <c r="E15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="36" t="s">
         <v>922</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -5325,12 +5441,12 @@
       <c r="E16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="35" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -5343,12 +5459,12 @@
       <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="35" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -5361,12 +5477,12 @@
       <c r="E18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="35" t="s">
         <v>925</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B19" s="1"/>
@@ -5379,12 +5495,12 @@
       <c r="E19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="35" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B20" s="1"/>
@@ -5397,12 +5513,12 @@
       <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="35" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B21" s="1"/>
@@ -5415,12 +5531,12 @@
       <c r="E21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="35" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B22" s="1"/>
@@ -5433,12 +5549,12 @@
       <c r="E22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="35" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B23" s="1"/>
@@ -5451,12 +5567,12 @@
       <c r="E23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="35" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B24" s="1"/>
@@ -5469,12 +5585,12 @@
       <c r="E24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="35" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B25" s="1"/>
@@ -5487,12 +5603,12 @@
       <c r="E25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="35" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B26" s="1"/>
@@ -5505,12 +5621,12 @@
       <c r="E26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="35" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="27" t="s">
         <v>892</v>
       </c>
       <c r="B27" s="1"/>
@@ -5523,12 +5639,12 @@
       <c r="E27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="35" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="28" t="s">
         <v>892</v>
       </c>
       <c r="B28" s="3"/>
@@ -5541,12 +5657,12 @@
       <c r="E28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="36" t="s">
         <v>936</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="28" t="s">
         <v>892</v>
       </c>
       <c r="B29" s="3"/>
@@ -5559,12 +5675,12 @@
       <c r="E29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="36" t="s">
         <v>938</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="29" t="s">
         <v>892</v>
       </c>
       <c r="B30" s="5"/>
@@ -5577,28 +5693,31 @@
       <c r="E30" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="37" t="s">
         <v>941</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="33" t="s">
         <v>892</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="1" t="s">
+      <c r="C31" s="40"/>
+      <c r="D31" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1" t="s">
+      <c r="E31" s="34"/>
+      <c r="F31" s="41" t="s">
         <v>180</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>